<commit_message>
Poprawka dla dokumentacji projektu
Poprawka dla dokumentacji projektu

Co-Authored-By: anusiahinz <anusiahinz@users.noreply.github.com>
Co-Authored-By: piotr9955 <piotr9955@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/DOKUMENTACJA/Harmonogram.xlsx
+++ b/DOKUMENTACJA/Harmonogram.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F605E4E4-14FC-4575-A48A-3A8460BD3FDB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366F66DF-E835-4EFC-A88C-442C7293AEC9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Lp</t>
   </si>
@@ -49,18 +49,6 @@
     <t>4. Ogłoszenia o pracę</t>
   </si>
   <si>
-    <t>5. Wnioski o urlop</t>
-  </si>
-  <si>
-    <t>6. Testy</t>
-  </si>
-  <si>
-    <t>7. Wdrożenie</t>
-  </si>
-  <si>
-    <t>8. Dokumentacja</t>
-  </si>
-  <si>
     <t>Harmonogram</t>
   </si>
   <si>
@@ -121,19 +109,16 @@
     <t>27.05.2018r.</t>
   </si>
   <si>
-    <t>03.06.2018r.</t>
-  </si>
-  <si>
     <t>10.06.2018r.</t>
   </si>
   <si>
     <t>Wykonanie testów całości aplikacji</t>
   </si>
   <si>
-    <t>Stworzenie dokumentacji</t>
-  </si>
-  <si>
-    <t>Moduł zarządzania wnioskami o urlop</t>
+    <t>5. Testy</t>
+  </si>
+  <si>
+    <t>6. Wdrożenie</t>
   </si>
 </sst>
 </file>
@@ -270,50 +255,50 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,254 +607,228 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="14"/>
+    </row>
+    <row r="16" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="15" t="s">
+      <c r="C17" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="15"/>
-    </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>15</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="13"/>
+      <c r="D17" s="13"/>
     </row>
   </sheetData>
-  <sortState ref="B3:D19">
-    <sortCondition ref="C3:C19"/>
+  <sortState ref="B3:D17">
+    <sortCondition ref="C3:C17"/>
   </sortState>
   <mergeCells count="6">
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="D4:D6"/>
   </mergeCells>

</xml_diff>